<commit_message>
updated spreadsheet and overlay based on EA feedback.
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-oracle-database-12c-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-oracle-database-12c-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-oracle-database-12c-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E55B7B6B-5056-4480-B55C-3F3C2E139E5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5D15192E-CAC9-1846-BC80-2AE3ECEC734D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-oracle-dat" sheetId="1" r:id="rId1"/>
@@ -11273,6 +11273,60 @@
     </r>
   </si>
   <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>(not in ARS)_x000B_Add to Overlay:_x000B_desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not mandatory in CMS ARS 3.1'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-000366
+The organization implements the security configuration settings.
+NIST SP 800-53 :: CM-6 b
+NIST SP 800-53A :: CM-6.1 (iv)
+NIST SP 800-53 Revision 4 :: CM-6 b 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CCI-000167
+The organization retains audit records for an organization-defined time period to provide support for after-the-fact investigations of security incidents and to meet regulatory and organizational information retention requirements.
+NIST SP 800-53 :: AU-11
+NIST SP 800-53A :: AU-11
+NIST SP 800-53 Revision 4 :: AU-11
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -11299,12 +11353,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">AU-11
+      <t xml:space="preserve">CCI-001547
+The organization defines the frequency on which it will review information system accounts for compliance with account management requirements.
+NIST SP 800-53 :: AC-2
+NIST SP 800-53A :: AC-2
+NIST SP 800-53 Revision 4 :: AC-2
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -11342,13 +11399,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">AC-2
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
+      <t>CCI-000148
+The organization reviews and analyzes information system audit records on an organization-defined frequency for indications of organization-defined inappropriate or unusual activity.
+NIST SP 800-53 :: AU-6 
+NIST SP 800-53A :: AU-6
+NIST SP 800-53 Revision 4 :: AU-6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -11356,39 +11418,8 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">CCI-000366
-The organization implements the security configuration settings.
-NIST SP 800-53 :: CM-6 b
-NIST SP 800-53A :: CM-6.1 (iv)
-NIST SP 800-53 Revision 4 :: CM-6 b
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AU-6</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+    <r>
+      <rPr>
         <strike/>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
@@ -11399,24 +11430,6 @@
       <t xml:space="preserve">
 </t>
     </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>(not in ARS)_x000B_Add to Overlay:_x000B_desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not mandatory in CMS ARS 3.1'</t>
   </si>
   <si>
     <r>
@@ -11441,11 +11454,25 @@
         <b/>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">SC-23
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">CCI-001184
+The information system protects the authenticity of communications sessions.
+NIST SP 800-53 :: SC-23
+NIST SP 800-53A :: SC-23 
+NIST SP 800-53 Revision 4 :: SC-23
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
   </si>
@@ -11454,7 +11481,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -11629,6 +11656,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="34">
@@ -12382,27 +12415,27 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B158" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="56.19921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.84765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.84765625" style="1"/>
+    <col min="8" max="8" width="19.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -12428,7 +12461,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="187.2">
+    <row r="2" spans="1:8" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -12448,11 +12481,11 @@
         <v>1100</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="409.5">
+    <row r="3" spans="1:8" ht="409.6">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -12476,7 +12509,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="202.8">
+    <row r="4" spans="1:8" ht="221">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -12500,7 +12533,7 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="218.4">
+    <row r="5" spans="1:8" ht="255">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
@@ -12524,7 +12557,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="409.5">
+    <row r="6" spans="1:8" ht="409.6">
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
@@ -12548,7 +12581,7 @@
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="327.60000000000002">
+    <row r="7" spans="1:8" ht="356">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -12572,7 +12605,7 @@
       </c>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="171.6">
+    <row r="8" spans="1:8" ht="204">
       <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
@@ -12596,7 +12629,7 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="187.2">
+    <row r="9" spans="1:8" ht="221">
       <c r="A9" s="6" t="s">
         <v>42</v>
       </c>
@@ -12620,7 +12653,7 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="171.6">
+    <row r="10" spans="1:8" ht="204">
       <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
@@ -12644,7 +12677,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="409.5">
+    <row r="11" spans="1:8" ht="409.6">
       <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
@@ -12668,7 +12701,7 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="296.39999999999998">
+    <row r="12" spans="1:8" ht="323">
       <c r="A12" s="6" t="s">
         <v>58</v>
       </c>
@@ -12692,7 +12725,7 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="409.5">
+    <row r="13" spans="1:8" ht="409.6">
       <c r="A13" s="6" t="s">
         <v>63</v>
       </c>
@@ -12716,7 +12749,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="187.2">
+    <row r="14" spans="1:8" ht="204">
       <c r="A14" s="6" t="s">
         <v>68</v>
       </c>
@@ -12740,7 +12773,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="409.5">
+    <row r="15" spans="1:8" ht="409.6">
       <c r="A15" s="6" t="s">
         <v>73</v>
       </c>
@@ -12764,7 +12797,7 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="409.5">
+    <row r="16" spans="1:8" ht="409.6">
       <c r="A16" s="6" t="s">
         <v>78</v>
       </c>
@@ -12788,7 +12821,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="409.5">
+    <row r="17" spans="1:8" ht="409.6">
       <c r="A17" s="6" t="s">
         <v>83</v>
       </c>
@@ -12812,7 +12845,7 @@
       </c>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="171.6">
+    <row r="18" spans="1:8" ht="204">
       <c r="A18" s="6" t="s">
         <v>88</v>
       </c>
@@ -12836,7 +12869,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="405.6">
+    <row r="19" spans="1:8" ht="409.6">
       <c r="A19" s="6" t="s">
         <v>93</v>
       </c>
@@ -12860,7 +12893,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="171.6">
+    <row r="20" spans="1:8" ht="204">
       <c r="A20" s="7" t="s">
         <v>98</v>
       </c>
@@ -12884,7 +12917,7 @@
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="409.5">
+    <row r="21" spans="1:8" ht="409.6">
       <c r="A21" s="6" t="s">
         <v>101</v>
       </c>
@@ -12908,7 +12941,7 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="409.5">
+    <row r="22" spans="1:8" ht="409.6">
       <c r="A22" s="6" t="s">
         <v>106</v>
       </c>
@@ -12932,7 +12965,7 @@
       </c>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="249.6">
+    <row r="23" spans="1:8" ht="289">
       <c r="A23" s="7" t="s">
         <v>111</v>
       </c>
@@ -12956,7 +12989,7 @@
       </c>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="187.2">
+    <row r="24" spans="1:8" ht="409.6">
       <c r="A24" s="7" t="s">
         <v>115</v>
       </c>
@@ -12976,11 +13009,11 @@
         <v>117</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="187.2">
+    <row r="25" spans="1:8" ht="409.6">
       <c r="A25" s="7" t="s">
         <v>118</v>
       </c>
@@ -13000,7 +13033,7 @@
         <v>122</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="H25" s="4"/>
     </row>
@@ -13028,7 +13061,7 @@
       </c>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="409.5">
+    <row r="27" spans="1:8" ht="409.6">
       <c r="A27" s="6" t="s">
         <v>128</v>
       </c>
@@ -13052,7 +13085,7 @@
       </c>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="409.5">
+    <row r="28" spans="1:8" ht="409.6">
       <c r="A28" s="6" t="s">
         <v>133</v>
       </c>
@@ -13076,7 +13109,7 @@
       </c>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="390">
+    <row r="29" spans="1:8" ht="409.6">
       <c r="A29" s="6" t="s">
         <v>138</v>
       </c>
@@ -13100,7 +13133,7 @@
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="409.5">
+    <row r="30" spans="1:8" ht="409.6">
       <c r="A30" s="6" t="s">
         <v>143</v>
       </c>
@@ -13124,7 +13157,7 @@
       </c>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="218.4">
+    <row r="31" spans="1:8" ht="255">
       <c r="A31" s="6" t="s">
         <v>148</v>
       </c>
@@ -13148,7 +13181,7 @@
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="187.2">
+    <row r="32" spans="1:8" ht="238">
       <c r="A32" s="6" t="s">
         <v>153</v>
       </c>
@@ -13172,7 +13205,7 @@
       </c>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="358.8">
+    <row r="33" spans="1:8" ht="388">
       <c r="A33" s="7" t="s">
         <v>158</v>
       </c>
@@ -13196,7 +13229,7 @@
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="171.6">
+    <row r="34" spans="1:8" ht="204">
       <c r="A34" s="6" t="s">
         <v>161</v>
       </c>
@@ -13220,7 +13253,7 @@
       </c>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="296.39999999999998">
+    <row r="35" spans="1:8" ht="323">
       <c r="A35" s="6" t="s">
         <v>166</v>
       </c>
@@ -13244,7 +13277,7 @@
       </c>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="171.6">
+    <row r="36" spans="1:8" ht="204">
       <c r="A36" s="6" t="s">
         <v>171</v>
       </c>
@@ -13268,7 +13301,7 @@
       </c>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" ht="171.6">
+    <row r="37" spans="1:8" ht="204">
       <c r="A37" s="6" t="s">
         <v>176</v>
       </c>
@@ -13292,7 +13325,7 @@
       </c>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="312">
+    <row r="38" spans="1:8" ht="340">
       <c r="A38" s="6" t="s">
         <v>181</v>
       </c>
@@ -13316,7 +13349,7 @@
       </c>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="343.2">
+    <row r="39" spans="1:8" ht="372">
       <c r="A39" s="6" t="s">
         <v>186</v>
       </c>
@@ -13340,7 +13373,7 @@
       </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" ht="187.2">
+    <row r="40" spans="1:8" ht="221">
       <c r="A40" s="6" t="s">
         <v>191</v>
       </c>
@@ -13364,7 +13397,7 @@
       </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" ht="187.2">
+    <row r="41" spans="1:8" ht="221">
       <c r="A41" s="6" t="s">
         <v>196</v>
       </c>
@@ -13412,7 +13445,7 @@
       </c>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="171.6">
+    <row r="43" spans="1:8" ht="204">
       <c r="A43" s="6" t="s">
         <v>206</v>
       </c>
@@ -13436,7 +13469,7 @@
       </c>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" ht="409.5">
+    <row r="44" spans="1:8" ht="409.6">
       <c r="A44" s="6" t="s">
         <v>211</v>
       </c>
@@ -13460,7 +13493,7 @@
       </c>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" ht="171.6">
+    <row r="45" spans="1:8" ht="204">
       <c r="A45" s="6" t="s">
         <v>216</v>
       </c>
@@ -13484,7 +13517,7 @@
       </c>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" ht="234">
+    <row r="46" spans="1:8" ht="255">
       <c r="A46" s="7" t="s">
         <v>221</v>
       </c>
@@ -13508,7 +13541,7 @@
       </c>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" ht="218.4">
+    <row r="47" spans="1:8" ht="255">
       <c r="A47" s="6" t="s">
         <v>224</v>
       </c>
@@ -13532,7 +13565,7 @@
       </c>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" ht="409.5">
+    <row r="48" spans="1:8" ht="409.6">
       <c r="A48" s="6" t="s">
         <v>229</v>
       </c>
@@ -13556,7 +13589,7 @@
       </c>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:8" ht="171.6">
+    <row r="49" spans="1:8" ht="204">
       <c r="A49" s="6" t="s">
         <v>234</v>
       </c>
@@ -13580,7 +13613,7 @@
       </c>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:8" ht="409.5">
+    <row r="50" spans="1:8" ht="409.6">
       <c r="A50" s="6" t="s">
         <v>239</v>
       </c>
@@ -13604,7 +13637,7 @@
       </c>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="171.6">
+    <row r="51" spans="1:8" ht="204">
       <c r="A51" s="6" t="s">
         <v>244</v>
       </c>
@@ -13628,7 +13661,7 @@
       </c>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:8" ht="405.6">
+    <row r="52" spans="1:8" ht="409.6">
       <c r="A52" s="6" t="s">
         <v>249</v>
       </c>
@@ -13652,7 +13685,7 @@
       </c>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:8" ht="409.5">
+    <row r="53" spans="1:8" ht="409.6">
       <c r="A53" s="6" t="s">
         <v>254</v>
       </c>
@@ -13676,7 +13709,7 @@
       </c>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:8" ht="409.5">
+    <row r="54" spans="1:8" ht="409.6">
       <c r="A54" s="6" t="s">
         <v>259</v>
       </c>
@@ -13700,7 +13733,7 @@
       </c>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:8" ht="296.39999999999998">
+    <row r="55" spans="1:8" ht="340">
       <c r="A55" s="6" t="s">
         <v>265</v>
       </c>
@@ -13724,7 +13757,7 @@
       </c>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="1:8" ht="409.5">
+    <row r="56" spans="1:8" ht="409.6">
       <c r="A56" s="6" t="s">
         <v>271</v>
       </c>
@@ -13748,7 +13781,7 @@
       </c>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="1:8" ht="409.5">
+    <row r="57" spans="1:8" ht="409.6">
       <c r="A57" s="7" t="s">
         <v>277</v>
       </c>
@@ -13772,7 +13805,7 @@
       </c>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:8" ht="409.5">
+    <row r="58" spans="1:8" ht="409.6">
       <c r="A58" s="6" t="s">
         <v>282</v>
       </c>
@@ -13796,7 +13829,7 @@
       </c>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:8" ht="409.5">
+    <row r="59" spans="1:8" ht="409.6">
       <c r="A59" s="7" t="s">
         <v>288</v>
       </c>
@@ -13820,7 +13853,7 @@
       </c>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:8" ht="409.5">
+    <row r="60" spans="1:8" ht="409.6">
       <c r="A60" s="6" t="s">
         <v>290</v>
       </c>
@@ -13844,7 +13877,7 @@
       </c>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:8" ht="409.5">
+    <row r="61" spans="1:8" ht="409.6">
       <c r="A61" s="6" t="s">
         <v>296</v>
       </c>
@@ -13868,7 +13901,7 @@
       </c>
       <c r="H61" s="4"/>
     </row>
-    <row r="62" spans="1:8" ht="409.5">
+    <row r="62" spans="1:8" ht="409.6">
       <c r="A62" s="7" t="s">
         <v>302</v>
       </c>
@@ -13892,7 +13925,7 @@
       </c>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" ht="409.5">
+    <row r="63" spans="1:8" ht="409.6">
       <c r="A63" s="6" t="s">
         <v>305</v>
       </c>
@@ -13916,7 +13949,7 @@
       </c>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="1:8" ht="409.5">
+    <row r="64" spans="1:8" ht="409.6">
       <c r="A64" s="6" t="s">
         <v>311</v>
       </c>
@@ -13940,7 +13973,7 @@
       </c>
       <c r="H64" s="4"/>
     </row>
-    <row r="65" spans="1:8" ht="409.5">
+    <row r="65" spans="1:8" ht="409.6">
       <c r="A65" s="6" t="s">
         <v>317</v>
       </c>
@@ -13964,7 +13997,7 @@
       </c>
       <c r="H65" s="4"/>
     </row>
-    <row r="66" spans="1:8" ht="409.5">
+    <row r="66" spans="1:8" ht="409.6">
       <c r="A66" s="6" t="s">
         <v>323</v>
       </c>
@@ -13988,7 +14021,7 @@
       </c>
       <c r="H66" s="4"/>
     </row>
-    <row r="67" spans="1:8" ht="409.5">
+    <row r="67" spans="1:8" ht="409.6">
       <c r="A67" s="6" t="s">
         <v>329</v>
       </c>
@@ -14012,7 +14045,7 @@
       </c>
       <c r="H67" s="4"/>
     </row>
-    <row r="68" spans="1:8" ht="409.5">
+    <row r="68" spans="1:8" ht="409.6">
       <c r="A68" s="6" t="s">
         <v>335</v>
       </c>
@@ -14036,7 +14069,7 @@
       </c>
       <c r="H68" s="4"/>
     </row>
-    <row r="69" spans="1:8" ht="409.5">
+    <row r="69" spans="1:8" ht="409.6">
       <c r="A69" s="6" t="s">
         <v>341</v>
       </c>
@@ -14060,7 +14093,7 @@
       </c>
       <c r="H69" s="4"/>
     </row>
-    <row r="70" spans="1:8" ht="358.8">
+    <row r="70" spans="1:8" ht="404">
       <c r="A70" s="6" t="s">
         <v>346</v>
       </c>
@@ -14084,7 +14117,7 @@
       </c>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:8" ht="343.2">
+    <row r="71" spans="1:8" ht="388">
       <c r="A71" s="6" t="s">
         <v>351</v>
       </c>
@@ -14108,7 +14141,7 @@
       </c>
       <c r="H71" s="4"/>
     </row>
-    <row r="72" spans="1:8" ht="327.60000000000002">
+    <row r="72" spans="1:8" ht="388">
       <c r="A72" s="6" t="s">
         <v>356</v>
       </c>
@@ -14132,7 +14165,7 @@
       </c>
       <c r="H72" s="4"/>
     </row>
-    <row r="73" spans="1:8" ht="405.6">
+    <row r="73" spans="1:8" ht="409.6">
       <c r="A73" s="6" t="s">
         <v>361</v>
       </c>
@@ -14156,7 +14189,7 @@
       </c>
       <c r="H73" s="4"/>
     </row>
-    <row r="74" spans="1:8" ht="312">
+    <row r="74" spans="1:8" ht="372">
       <c r="A74" s="6" t="s">
         <v>365</v>
       </c>
@@ -14180,7 +14213,7 @@
       </c>
       <c r="H74" s="4"/>
     </row>
-    <row r="75" spans="1:8" ht="409.5">
+    <row r="75" spans="1:8" ht="409.6">
       <c r="A75" s="6" t="s">
         <v>370</v>
       </c>
@@ -14204,7 +14237,7 @@
       </c>
       <c r="H75" s="4"/>
     </row>
-    <row r="76" spans="1:8" ht="409.5">
+    <row r="76" spans="1:8" ht="409.6">
       <c r="A76" s="6" t="s">
         <v>375</v>
       </c>
@@ -14228,7 +14261,7 @@
       </c>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="1:8" ht="280.8">
+    <row r="77" spans="1:8" ht="323">
       <c r="A77" s="6" t="s">
         <v>380</v>
       </c>
@@ -14252,7 +14285,7 @@
       </c>
       <c r="H77" s="4"/>
     </row>
-    <row r="78" spans="1:8" ht="171.6">
+    <row r="78" spans="1:8" ht="204">
       <c r="A78" s="6" t="s">
         <v>385</v>
       </c>
@@ -14276,7 +14309,7 @@
       </c>
       <c r="H78" s="4"/>
     </row>
-    <row r="79" spans="1:8" ht="409.5">
+    <row r="79" spans="1:8" ht="409.6">
       <c r="A79" s="6" t="s">
         <v>390</v>
       </c>
@@ -14300,7 +14333,7 @@
       </c>
       <c r="H79" s="4"/>
     </row>
-    <row r="80" spans="1:8" ht="409.5">
+    <row r="80" spans="1:8" ht="409.6">
       <c r="A80" s="6" t="s">
         <v>395</v>
       </c>
@@ -14324,7 +14357,7 @@
       </c>
       <c r="H80" s="4"/>
     </row>
-    <row r="81" spans="1:8" ht="409.5">
+    <row r="81" spans="1:8" ht="409.6">
       <c r="A81" s="6" t="s">
         <v>400</v>
       </c>
@@ -14348,7 +14381,7 @@
       </c>
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="1:8" ht="409.5">
+    <row r="82" spans="1:8" ht="409.6">
       <c r="A82" s="7" t="s">
         <v>406</v>
       </c>
@@ -14372,7 +14405,7 @@
       </c>
       <c r="H82" s="4"/>
     </row>
-    <row r="83" spans="1:8" ht="409.5">
+    <row r="83" spans="1:8" ht="409.6">
       <c r="A83" s="7" t="s">
         <v>409</v>
       </c>
@@ -14396,7 +14429,7 @@
       </c>
       <c r="H83" s="4"/>
     </row>
-    <row r="84" spans="1:8" ht="409.5">
+    <row r="84" spans="1:8" ht="409.6">
       <c r="A84" s="6" t="s">
         <v>412</v>
       </c>
@@ -14420,7 +14453,7 @@
       </c>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="1:8" ht="409.5">
+    <row r="85" spans="1:8" ht="409.6">
       <c r="A85" s="6" t="s">
         <v>418</v>
       </c>
@@ -14444,7 +14477,7 @@
       </c>
       <c r="H85" s="4"/>
     </row>
-    <row r="86" spans="1:8" ht="409.5">
+    <row r="86" spans="1:8" ht="409.6">
       <c r="A86" s="6" t="s">
         <v>422</v>
       </c>
@@ -14468,7 +14501,7 @@
       </c>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="1:8" ht="390">
+    <row r="87" spans="1:8" ht="409.6">
       <c r="A87" s="6" t="s">
         <v>427</v>
       </c>
@@ -14492,7 +14525,7 @@
       </c>
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="1:8" ht="409.5">
+    <row r="88" spans="1:8" ht="409.6">
       <c r="A88" s="7" t="s">
         <v>432</v>
       </c>
@@ -14516,7 +14549,7 @@
       </c>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="1:8" ht="409.5">
+    <row r="89" spans="1:8" ht="409.6">
       <c r="A89" s="6" t="s">
         <v>436</v>
       </c>
@@ -14540,7 +14573,7 @@
       </c>
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="1:8" ht="409.5">
+    <row r="90" spans="1:8" ht="409.6">
       <c r="A90" s="7" t="s">
         <v>442</v>
       </c>
@@ -14564,7 +14597,7 @@
       </c>
       <c r="H90" s="4"/>
     </row>
-    <row r="91" spans="1:8" ht="409.5">
+    <row r="91" spans="1:8" ht="409.6">
       <c r="A91" s="6" t="s">
         <v>444</v>
       </c>
@@ -14588,7 +14621,7 @@
       </c>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:8" ht="409.5">
+    <row r="92" spans="1:8" ht="409.6">
       <c r="A92" s="6" t="s">
         <v>450</v>
       </c>
@@ -14636,7 +14669,7 @@
       </c>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="1:8" ht="409.5">
+    <row r="94" spans="1:8" ht="409.6">
       <c r="A94" s="6" t="s">
         <v>461</v>
       </c>
@@ -14660,7 +14693,7 @@
       </c>
       <c r="H94" s="4"/>
     </row>
-    <row r="95" spans="1:8" ht="409.5">
+    <row r="95" spans="1:8" ht="409.6">
       <c r="A95" s="6" t="s">
         <v>467</v>
       </c>
@@ -14684,7 +14717,7 @@
       </c>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="1:8" ht="409.5">
+    <row r="96" spans="1:8" ht="409.6">
       <c r="A96" s="6" t="s">
         <v>473</v>
       </c>
@@ -14708,7 +14741,7 @@
       </c>
       <c r="H96" s="4"/>
     </row>
-    <row r="97" spans="1:8" ht="409.5">
+    <row r="97" spans="1:8" ht="409.6">
       <c r="A97" s="6" t="s">
         <v>479</v>
       </c>
@@ -14732,7 +14765,7 @@
       </c>
       <c r="H97" s="4"/>
     </row>
-    <row r="98" spans="1:8" ht="409.5">
+    <row r="98" spans="1:8" ht="409.6">
       <c r="A98" s="6" t="s">
         <v>485</v>
       </c>
@@ -14756,7 +14789,7 @@
       </c>
       <c r="H98" s="4"/>
     </row>
-    <row r="99" spans="1:8" ht="409.5">
+    <row r="99" spans="1:8" ht="409.6">
       <c r="A99" s="6" t="s">
         <v>491</v>
       </c>
@@ -14780,7 +14813,7 @@
       </c>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="1:8" ht="296.39999999999998">
+    <row r="100" spans="1:8" ht="323">
       <c r="A100" s="6" t="s">
         <v>497</v>
       </c>
@@ -14804,7 +14837,7 @@
       </c>
       <c r="H100" s="4"/>
     </row>
-    <row r="101" spans="1:8" ht="409.5">
+    <row r="101" spans="1:8" ht="409.6">
       <c r="A101" s="6" t="s">
         <v>503</v>
       </c>
@@ -14828,7 +14861,7 @@
       </c>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" spans="1:8" ht="409.5">
+    <row r="102" spans="1:8" ht="409.6">
       <c r="A102" s="6" t="s">
         <v>509</v>
       </c>
@@ -14852,7 +14885,7 @@
       </c>
       <c r="H102" s="4"/>
     </row>
-    <row r="103" spans="1:8" ht="409.5">
+    <row r="103" spans="1:8" ht="409.6">
       <c r="A103" s="6" t="s">
         <v>514</v>
       </c>
@@ -14876,7 +14909,7 @@
       </c>
       <c r="H103" s="4"/>
     </row>
-    <row r="104" spans="1:8" ht="409.5">
+    <row r="104" spans="1:8" ht="409.6">
       <c r="A104" s="6" t="s">
         <v>520</v>
       </c>
@@ -14900,7 +14933,7 @@
       </c>
       <c r="H104" s="4"/>
     </row>
-    <row r="105" spans="1:8" ht="409.5">
+    <row r="105" spans="1:8" ht="409.6">
       <c r="A105" s="6" t="s">
         <v>526</v>
       </c>
@@ -14924,7 +14957,7 @@
       </c>
       <c r="H105" s="4"/>
     </row>
-    <row r="106" spans="1:8" ht="409.5">
+    <row r="106" spans="1:8" ht="409.6">
       <c r="A106" s="6" t="s">
         <v>532</v>
       </c>
@@ -14948,7 +14981,7 @@
       </c>
       <c r="H106" s="4"/>
     </row>
-    <row r="107" spans="1:8" ht="405.6">
+    <row r="107" spans="1:8" ht="409.6">
       <c r="A107" s="6" t="s">
         <v>538</v>
       </c>
@@ -14972,7 +15005,7 @@
       </c>
       <c r="H107" s="4"/>
     </row>
-    <row r="108" spans="1:8" ht="409.5">
+    <row r="108" spans="1:8" ht="409.6">
       <c r="A108" s="6" t="s">
         <v>544</v>
       </c>
@@ -14996,7 +15029,7 @@
       </c>
       <c r="H108" s="4"/>
     </row>
-    <row r="109" spans="1:8" ht="280.8">
+    <row r="109" spans="1:8" ht="306">
       <c r="A109" s="6" t="s">
         <v>550</v>
       </c>
@@ -15020,7 +15053,7 @@
       </c>
       <c r="H109" s="4"/>
     </row>
-    <row r="110" spans="1:8" ht="409.5">
+    <row r="110" spans="1:8" ht="409.6">
       <c r="A110" s="6" t="s">
         <v>556</v>
       </c>
@@ -15044,7 +15077,7 @@
       </c>
       <c r="H110" s="4"/>
     </row>
-    <row r="111" spans="1:8" ht="409.5">
+    <row r="111" spans="1:8" ht="409.6">
       <c r="A111" s="6" t="s">
         <v>562</v>
       </c>
@@ -15068,7 +15101,7 @@
       </c>
       <c r="H111" s="4"/>
     </row>
-    <row r="112" spans="1:8" ht="343.2">
+    <row r="112" spans="1:8" ht="372">
       <c r="A112" s="6" t="s">
         <v>568</v>
       </c>
@@ -15092,7 +15125,7 @@
       </c>
       <c r="H112" s="4"/>
     </row>
-    <row r="113" spans="1:8" ht="374.4">
+    <row r="113" spans="1:8" ht="409.6">
       <c r="A113" s="6" t="s">
         <v>574</v>
       </c>
@@ -15116,7 +15149,7 @@
       </c>
       <c r="H113" s="4"/>
     </row>
-    <row r="114" spans="1:8" ht="265.2">
+    <row r="114" spans="1:8" ht="289">
       <c r="A114" s="7" t="s">
         <v>579</v>
       </c>
@@ -15140,7 +15173,7 @@
       </c>
       <c r="H114" s="4"/>
     </row>
-    <row r="115" spans="1:8" ht="409.5">
+    <row r="115" spans="1:8" ht="409.6">
       <c r="A115" s="6" t="s">
         <v>583</v>
       </c>
@@ -15164,7 +15197,7 @@
       </c>
       <c r="H115" s="4"/>
     </row>
-    <row r="116" spans="1:8" ht="409.5">
+    <row r="116" spans="1:8" ht="409.6">
       <c r="A116" s="6" t="s">
         <v>589</v>
       </c>
@@ -15188,7 +15221,7 @@
       </c>
       <c r="H116" s="4"/>
     </row>
-    <row r="117" spans="1:8" ht="409.5">
+    <row r="117" spans="1:8" ht="409.6">
       <c r="A117" s="6" t="s">
         <v>594</v>
       </c>
@@ -15212,7 +15245,7 @@
       </c>
       <c r="H117" s="4"/>
     </row>
-    <row r="118" spans="1:8" ht="409.5">
+    <row r="118" spans="1:8" ht="409.6">
       <c r="A118" s="6" t="s">
         <v>599</v>
       </c>
@@ -15236,7 +15269,7 @@
       </c>
       <c r="H118" s="4"/>
     </row>
-    <row r="119" spans="1:8" ht="409.5">
+    <row r="119" spans="1:8" ht="409.6">
       <c r="A119" s="6" t="s">
         <v>604</v>
       </c>
@@ -15260,7 +15293,7 @@
       </c>
       <c r="H119" s="4"/>
     </row>
-    <row r="120" spans="1:8" ht="409.5">
+    <row r="120" spans="1:8" ht="409.6">
       <c r="A120" s="7" t="s">
         <v>609</v>
       </c>
@@ -15284,7 +15317,7 @@
       </c>
       <c r="H120" s="4"/>
     </row>
-    <row r="121" spans="1:8" ht="409.5">
+    <row r="121" spans="1:8" ht="409.6">
       <c r="A121" s="6" t="s">
         <v>614</v>
       </c>
@@ -15308,7 +15341,7 @@
       </c>
       <c r="H121" s="4"/>
     </row>
-    <row r="122" spans="1:8" ht="343.2">
+    <row r="122" spans="1:8" ht="372">
       <c r="A122" s="7" t="s">
         <v>620</v>
       </c>
@@ -15332,7 +15365,7 @@
       </c>
       <c r="H122" s="4"/>
     </row>
-    <row r="123" spans="1:8" ht="409.5">
+    <row r="123" spans="1:8" ht="409.6">
       <c r="A123" s="7" t="s">
         <v>625</v>
       </c>
@@ -15356,7 +15389,7 @@
       </c>
       <c r="H123" s="4"/>
     </row>
-    <row r="124" spans="1:8" ht="343.2">
+    <row r="124" spans="1:8" ht="404">
       <c r="A124" s="7" t="s">
         <v>629</v>
       </c>
@@ -15380,7 +15413,7 @@
       </c>
       <c r="H124" s="4"/>
     </row>
-    <row r="125" spans="1:8" ht="409.5">
+    <row r="125" spans="1:8" ht="409.6">
       <c r="A125" s="7" t="s">
         <v>633</v>
       </c>
@@ -15404,7 +15437,7 @@
       </c>
       <c r="H125" s="4"/>
     </row>
-    <row r="126" spans="1:8" ht="280.8">
+    <row r="126" spans="1:8" ht="340">
       <c r="A126" s="6" t="s">
         <v>637</v>
       </c>
@@ -15428,7 +15461,7 @@
       </c>
       <c r="H126" s="4"/>
     </row>
-    <row r="127" spans="1:8" ht="409.5">
+    <row r="127" spans="1:8" ht="409.6">
       <c r="A127" s="7" t="s">
         <v>643</v>
       </c>
@@ -15452,7 +15485,7 @@
       </c>
       <c r="H127" s="4"/>
     </row>
-    <row r="128" spans="1:8" ht="409.5">
+    <row r="128" spans="1:8" ht="409.6">
       <c r="A128" s="7" t="s">
         <v>647</v>
       </c>
@@ -15476,7 +15509,7 @@
       </c>
       <c r="H128" s="4"/>
     </row>
-    <row r="129" spans="1:8" ht="409.5">
+    <row r="129" spans="1:8" ht="409.6">
       <c r="A129" s="7" t="s">
         <v>652</v>
       </c>
@@ -15500,7 +15533,7 @@
       </c>
       <c r="H129" s="4"/>
     </row>
-    <row r="130" spans="1:8" ht="409.5">
+    <row r="130" spans="1:8" ht="409.6">
       <c r="A130" s="7" t="s">
         <v>657</v>
       </c>
@@ -15524,7 +15557,7 @@
       </c>
       <c r="H130" s="4"/>
     </row>
-    <row r="131" spans="1:8" ht="409.5">
+    <row r="131" spans="1:8" ht="409.6">
       <c r="A131" s="7" t="s">
         <v>662</v>
       </c>
@@ -15548,7 +15581,7 @@
       </c>
       <c r="H131" s="4"/>
     </row>
-    <row r="132" spans="1:8" ht="409.5">
+    <row r="132" spans="1:8" ht="409.6">
       <c r="A132" s="7" t="s">
         <v>667</v>
       </c>
@@ -15572,7 +15605,7 @@
       </c>
       <c r="H132" s="4"/>
     </row>
-    <row r="133" spans="1:8" ht="409.5">
+    <row r="133" spans="1:8" ht="409.6">
       <c r="A133" s="7" t="s">
         <v>672</v>
       </c>
@@ -15596,7 +15629,7 @@
       </c>
       <c r="H133" s="4"/>
     </row>
-    <row r="134" spans="1:8" ht="409.5">
+    <row r="134" spans="1:8" ht="409.6">
       <c r="A134" s="7" t="s">
         <v>677</v>
       </c>
@@ -15620,7 +15653,7 @@
       </c>
       <c r="H134" s="4"/>
     </row>
-    <row r="135" spans="1:8" ht="409.5">
+    <row r="135" spans="1:8" ht="409.6">
       <c r="A135" s="7" t="s">
         <v>680</v>
       </c>
@@ -15644,7 +15677,7 @@
       </c>
       <c r="H135" s="4"/>
     </row>
-    <row r="136" spans="1:8" ht="409.5">
+    <row r="136" spans="1:8" ht="409.6">
       <c r="A136" s="7" t="s">
         <v>684</v>
       </c>
@@ -15668,7 +15701,7 @@
       </c>
       <c r="H136" s="4"/>
     </row>
-    <row r="137" spans="1:8" ht="343.2">
+    <row r="137" spans="1:8" ht="388">
       <c r="A137" s="7" t="s">
         <v>688</v>
       </c>
@@ -15692,7 +15725,7 @@
       </c>
       <c r="H137" s="4"/>
     </row>
-    <row r="138" spans="1:8" ht="374.4">
+    <row r="138" spans="1:8" ht="404">
       <c r="A138" s="7" t="s">
         <v>693</v>
       </c>
@@ -15716,7 +15749,7 @@
       </c>
       <c r="H138" s="4"/>
     </row>
-    <row r="139" spans="1:8" ht="343.2">
+    <row r="139" spans="1:8" ht="388">
       <c r="A139" s="7" t="s">
         <v>698</v>
       </c>
@@ -15740,7 +15773,7 @@
       </c>
       <c r="H139" s="4"/>
     </row>
-    <row r="140" spans="1:8" ht="343.2">
+    <row r="140" spans="1:8" ht="388">
       <c r="A140" s="7" t="s">
         <v>702</v>
       </c>
@@ -15764,7 +15797,7 @@
       </c>
       <c r="H140" s="4"/>
     </row>
-    <row r="141" spans="1:8" ht="409.5">
+    <row r="141" spans="1:8" ht="409.6">
       <c r="A141" s="7" t="s">
         <v>706</v>
       </c>
@@ -15788,7 +15821,7 @@
       </c>
       <c r="H141" s="4"/>
     </row>
-    <row r="142" spans="1:8" ht="409.5">
+    <row r="142" spans="1:8" ht="409.6">
       <c r="A142" s="6" t="s">
         <v>710</v>
       </c>
@@ -15812,7 +15845,7 @@
       </c>
       <c r="H142" s="4"/>
     </row>
-    <row r="143" spans="1:8" ht="409.5">
+    <row r="143" spans="1:8" ht="409.6">
       <c r="A143" s="7" t="s">
         <v>716</v>
       </c>
@@ -15836,7 +15869,7 @@
       </c>
       <c r="H143" s="4"/>
     </row>
-    <row r="144" spans="1:8" ht="409.5">
+    <row r="144" spans="1:8" ht="409.6">
       <c r="A144" s="6" t="s">
         <v>718</v>
       </c>
@@ -15860,7 +15893,7 @@
       </c>
       <c r="H144" s="4"/>
     </row>
-    <row r="145" spans="1:8" ht="409.5">
+    <row r="145" spans="1:8" ht="409.6">
       <c r="A145" s="7" t="s">
         <v>723</v>
       </c>
@@ -15884,7 +15917,7 @@
       </c>
       <c r="H145" s="4"/>
     </row>
-    <row r="146" spans="1:8" ht="409.5">
+    <row r="146" spans="1:8" ht="409.6">
       <c r="A146" s="6" t="s">
         <v>726</v>
       </c>
@@ -15908,7 +15941,7 @@
       </c>
       <c r="H146" s="4"/>
     </row>
-    <row r="147" spans="1:8" ht="409.5">
+    <row r="147" spans="1:8" ht="409.6">
       <c r="A147" s="6" t="s">
         <v>732</v>
       </c>
@@ -15932,7 +15965,7 @@
       </c>
       <c r="H147" s="4"/>
     </row>
-    <row r="148" spans="1:8" ht="343.2">
+    <row r="148" spans="1:8" ht="388">
       <c r="A148" s="7" t="s">
         <v>738</v>
       </c>
@@ -15956,7 +15989,7 @@
       </c>
       <c r="H148" s="4"/>
     </row>
-    <row r="149" spans="1:8" ht="409.5">
+    <row r="149" spans="1:8" ht="409.6">
       <c r="A149" s="6" t="s">
         <v>739</v>
       </c>
@@ -15980,12 +16013,12 @@
       </c>
       <c r="H149" s="4"/>
     </row>
-    <row r="150" spans="1:8" ht="390">
+    <row r="150" spans="1:8" ht="409.6">
       <c r="A150" s="7" t="s">
         <v>744</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>745</v>
@@ -16003,10 +16036,10 @@
         <v>749</v>
       </c>
       <c r="H150" s="10" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" ht="327.60000000000002">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="388">
       <c r="A151" s="6" t="s">
         <v>750</v>
       </c>
@@ -16030,7 +16063,7 @@
       </c>
       <c r="H151" s="4"/>
     </row>
-    <row r="152" spans="1:8" ht="409.5">
+    <row r="152" spans="1:8" ht="409.6">
       <c r="A152" s="6" t="s">
         <v>756</v>
       </c>
@@ -16054,12 +16087,12 @@
       </c>
       <c r="H152" s="4"/>
     </row>
-    <row r="153" spans="1:8" ht="409.5">
+    <row r="153" spans="1:8" ht="409.6">
       <c r="A153" s="7" t="s">
         <v>761</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>762</v>
@@ -16077,10 +16110,10 @@
         <v>766</v>
       </c>
       <c r="H153" s="10" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" ht="409.5">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="409.6">
       <c r="A154" s="7" t="s">
         <v>767</v>
       </c>
@@ -16104,7 +16137,7 @@
       </c>
       <c r="H154" s="4"/>
     </row>
-    <row r="155" spans="1:8" ht="409.5">
+    <row r="155" spans="1:8" ht="409.6">
       <c r="A155" s="6" t="s">
         <v>770</v>
       </c>
@@ -16128,7 +16161,7 @@
       </c>
       <c r="H155" s="4"/>
     </row>
-    <row r="156" spans="1:8" ht="409.5">
+    <row r="156" spans="1:8" ht="409.6">
       <c r="A156" s="6" t="s">
         <v>776</v>
       </c>
@@ -16152,7 +16185,7 @@
       </c>
       <c r="H156" s="4"/>
     </row>
-    <row r="157" spans="1:8" ht="409.5">
+    <row r="157" spans="1:8" ht="409.6">
       <c r="A157" s="6" t="s">
         <v>781</v>
       </c>
@@ -16176,7 +16209,7 @@
       </c>
       <c r="H157" s="4"/>
     </row>
-    <row r="158" spans="1:8" ht="409.5">
+    <row r="158" spans="1:8" ht="409.6">
       <c r="A158" s="7" t="s">
         <v>786</v>
       </c>
@@ -16200,7 +16233,7 @@
       </c>
       <c r="H158" s="4"/>
     </row>
-    <row r="159" spans="1:8" ht="409.5">
+    <row r="159" spans="1:8" ht="409.6">
       <c r="A159" s="6" t="s">
         <v>791</v>
       </c>
@@ -16224,7 +16257,7 @@
       </c>
       <c r="H159" s="4"/>
     </row>
-    <row r="160" spans="1:8" ht="409.5">
+    <row r="160" spans="1:8" ht="409.6">
       <c r="A160" s="6" t="s">
         <v>797</v>
       </c>
@@ -16248,7 +16281,7 @@
       </c>
       <c r="H160" s="4"/>
     </row>
-    <row r="161" spans="1:8" ht="358.8">
+    <row r="161" spans="1:8" ht="388">
       <c r="A161" s="6" t="s">
         <v>803</v>
       </c>
@@ -16272,7 +16305,7 @@
       </c>
       <c r="H161" s="4"/>
     </row>
-    <row r="162" spans="1:8" ht="409.5">
+    <row r="162" spans="1:8" ht="409.6">
       <c r="A162" s="7" t="s">
         <v>809</v>
       </c>
@@ -16296,7 +16329,7 @@
       </c>
       <c r="H162" s="4"/>
     </row>
-    <row r="163" spans="1:8" ht="409.5">
+    <row r="163" spans="1:8" ht="409.6">
       <c r="A163" s="6" t="s">
         <v>811</v>
       </c>
@@ -16320,7 +16353,7 @@
       </c>
       <c r="H163" s="4"/>
     </row>
-    <row r="164" spans="1:8" ht="409.5">
+    <row r="164" spans="1:8" ht="409.6">
       <c r="A164" s="6" t="s">
         <v>817</v>
       </c>
@@ -16344,7 +16377,7 @@
       </c>
       <c r="H164" s="4"/>
     </row>
-    <row r="165" spans="1:8" ht="409.5">
+    <row r="165" spans="1:8" ht="409.6">
       <c r="A165" s="6" t="s">
         <v>823</v>
       </c>
@@ -16368,7 +16401,7 @@
       </c>
       <c r="H165" s="4"/>
     </row>
-    <row r="166" spans="1:8" ht="409.5">
+    <row r="166" spans="1:8" ht="409.6">
       <c r="A166" s="6" t="s">
         <v>829</v>
       </c>
@@ -16392,7 +16425,7 @@
       </c>
       <c r="H166" s="4"/>
     </row>
-    <row r="167" spans="1:8" ht="327.60000000000002">
+    <row r="167" spans="1:8" ht="356">
       <c r="A167" s="6" t="s">
         <v>835</v>
       </c>
@@ -16416,7 +16449,7 @@
       </c>
       <c r="H167" s="4"/>
     </row>
-    <row r="168" spans="1:8" ht="409.5">
+    <row r="168" spans="1:8" ht="409.6">
       <c r="A168" s="6" t="s">
         <v>841</v>
       </c>
@@ -16440,7 +16473,7 @@
       </c>
       <c r="H168" s="4"/>
     </row>
-    <row r="169" spans="1:8" ht="409.5">
+    <row r="169" spans="1:8" ht="409.6">
       <c r="A169" s="6" t="s">
         <v>846</v>
       </c>
@@ -16464,7 +16497,7 @@
       </c>
       <c r="H169" s="4"/>
     </row>
-    <row r="170" spans="1:8" ht="409.5">
+    <row r="170" spans="1:8" ht="409.6">
       <c r="A170" s="6" t="s">
         <v>852</v>
       </c>
@@ -16488,7 +16521,7 @@
       </c>
       <c r="H170" s="4"/>
     </row>
-    <row r="171" spans="1:8" ht="358.8">
+    <row r="171" spans="1:8" ht="404">
       <c r="A171" s="6" t="s">
         <v>858</v>
       </c>
@@ -16512,7 +16545,7 @@
       </c>
       <c r="H171" s="4"/>
     </row>
-    <row r="172" spans="1:8" ht="409.5">
+    <row r="172" spans="1:8" ht="409.6">
       <c r="A172" s="6" t="s">
         <v>864</v>
       </c>
@@ -16536,7 +16569,7 @@
       </c>
       <c r="H172" s="4"/>
     </row>
-    <row r="173" spans="1:8" ht="409.5">
+    <row r="173" spans="1:8" ht="409.6">
       <c r="A173" s="6" t="s">
         <v>870</v>
       </c>
@@ -16560,7 +16593,7 @@
       </c>
       <c r="H173" s="4"/>
     </row>
-    <row r="174" spans="1:8" ht="409.5">
+    <row r="174" spans="1:8" ht="409.6">
       <c r="A174" s="6" t="s">
         <v>876</v>
       </c>
@@ -16584,7 +16617,7 @@
       </c>
       <c r="H174" s="4"/>
     </row>
-    <row r="175" spans="1:8" ht="409.5">
+    <row r="175" spans="1:8" ht="409.6">
       <c r="A175" s="6" t="s">
         <v>882</v>
       </c>
@@ -16608,7 +16641,7 @@
       </c>
       <c r="H175" s="4"/>
     </row>
-    <row r="176" spans="1:8" ht="409.5">
+    <row r="176" spans="1:8" ht="409.6">
       <c r="A176" s="6" t="s">
         <v>888</v>
       </c>
@@ -16632,7 +16665,7 @@
       </c>
       <c r="H176" s="4"/>
     </row>
-    <row r="177" spans="1:8" ht="374.4">
+    <row r="177" spans="1:8" ht="404">
       <c r="A177" s="6" t="s">
         <v>893</v>
       </c>
@@ -16656,7 +16689,7 @@
       </c>
       <c r="H177" s="4"/>
     </row>
-    <row r="178" spans="1:8" ht="409.5">
+    <row r="178" spans="1:8" ht="409.6">
       <c r="A178" s="7" t="s">
         <v>899</v>
       </c>
@@ -16680,7 +16713,7 @@
       </c>
       <c r="H178" s="4"/>
     </row>
-    <row r="179" spans="1:8" ht="409.5">
+    <row r="179" spans="1:8" ht="409.6">
       <c r="A179" s="6" t="s">
         <v>904</v>
       </c>
@@ -16704,7 +16737,7 @@
       </c>
       <c r="H179" s="4"/>
     </row>
-    <row r="180" spans="1:8" ht="409.5">
+    <row r="180" spans="1:8" ht="409.6">
       <c r="A180" s="6" t="s">
         <v>910</v>
       </c>
@@ -16728,7 +16761,7 @@
       </c>
       <c r="H180" s="4"/>
     </row>
-    <row r="181" spans="1:8" ht="409.5">
+    <row r="181" spans="1:8" ht="409.6">
       <c r="A181" s="6" t="s">
         <v>916</v>
       </c>
@@ -16752,7 +16785,7 @@
       </c>
       <c r="H181" s="4"/>
     </row>
-    <row r="182" spans="1:8" ht="409.5">
+    <row r="182" spans="1:8" ht="409.6">
       <c r="A182" s="6" t="s">
         <v>921</v>
       </c>
@@ -16776,7 +16809,7 @@
       </c>
       <c r="H182" s="4"/>
     </row>
-    <row r="183" spans="1:8" ht="409.5">
+    <row r="183" spans="1:8" ht="409.6">
       <c r="A183" s="6" t="s">
         <v>926</v>
       </c>
@@ -16800,7 +16833,7 @@
       </c>
       <c r="H183" s="4"/>
     </row>
-    <row r="184" spans="1:8" ht="409.5">
+    <row r="184" spans="1:8" ht="409.6">
       <c r="A184" s="6" t="s">
         <v>931</v>
       </c>
@@ -16824,7 +16857,7 @@
       </c>
       <c r="H184" s="4"/>
     </row>
-    <row r="185" spans="1:8" ht="409.5">
+    <row r="185" spans="1:8" ht="409.6">
       <c r="A185" s="6" t="s">
         <v>936</v>
       </c>
@@ -16848,7 +16881,7 @@
       </c>
       <c r="H185" s="4"/>
     </row>
-    <row r="186" spans="1:8" ht="312">
+    <row r="186" spans="1:8" ht="372">
       <c r="A186" s="6" t="s">
         <v>941</v>
       </c>
@@ -16872,7 +16905,7 @@
       </c>
       <c r="H186" s="4"/>
     </row>
-    <row r="187" spans="1:8" ht="409.5">
+    <row r="187" spans="1:8" ht="409.6">
       <c r="A187" s="6" t="s">
         <v>946</v>
       </c>
@@ -16896,7 +16929,7 @@
       </c>
       <c r="H187" s="4"/>
     </row>
-    <row r="188" spans="1:8" ht="374.4">
+    <row r="188" spans="1:8" ht="409.6">
       <c r="A188" s="6" t="s">
         <v>951</v>
       </c>
@@ -16920,7 +16953,7 @@
       </c>
       <c r="H188" s="4"/>
     </row>
-    <row r="189" spans="1:8" ht="409.5">
+    <row r="189" spans="1:8" ht="409.6">
       <c r="A189" s="6" t="s">
         <v>957</v>
       </c>
@@ -16944,7 +16977,7 @@
       </c>
       <c r="H189" s="4"/>
     </row>
-    <row r="190" spans="1:8" ht="374.4">
+    <row r="190" spans="1:8" ht="409.6">
       <c r="A190" s="6" t="s">
         <v>962</v>
       </c>
@@ -16968,7 +17001,7 @@
       </c>
       <c r="H190" s="4"/>
     </row>
-    <row r="191" spans="1:8" ht="280.8">
+    <row r="191" spans="1:8" ht="340">
       <c r="A191" s="6" t="s">
         <v>967</v>
       </c>
@@ -16992,7 +17025,7 @@
       </c>
       <c r="H191" s="4"/>
     </row>
-    <row r="192" spans="1:8" ht="265.2">
+    <row r="192" spans="1:8" ht="289">
       <c r="A192" s="6" t="s">
         <v>972</v>
       </c>
@@ -17016,7 +17049,7 @@
       </c>
       <c r="H192" s="4"/>
     </row>
-    <row r="193" spans="1:8" ht="390">
+    <row r="193" spans="1:8" ht="409.6">
       <c r="A193" s="6" t="s">
         <v>978</v>
       </c>
@@ -17040,7 +17073,7 @@
       </c>
       <c r="H193" s="4"/>
     </row>
-    <row r="194" spans="1:8" ht="409.5">
+    <row r="194" spans="1:8" ht="409.6">
       <c r="A194" s="6" t="s">
         <v>984</v>
       </c>
@@ -17064,7 +17097,7 @@
       </c>
       <c r="H194" s="4"/>
     </row>
-    <row r="195" spans="1:8" ht="409.5">
+    <row r="195" spans="1:8" ht="409.6">
       <c r="A195" s="6" t="s">
         <v>990</v>
       </c>
@@ -17088,7 +17121,7 @@
       </c>
       <c r="H195" s="4"/>
     </row>
-    <row r="196" spans="1:8" ht="409.5">
+    <row r="196" spans="1:8" ht="409.6">
       <c r="A196" s="6" t="s">
         <v>994</v>
       </c>
@@ -17112,7 +17145,7 @@
       </c>
       <c r="H196" s="4"/>
     </row>
-    <row r="197" spans="1:8" ht="171.6">
+    <row r="197" spans="1:8" ht="204">
       <c r="A197" s="6" t="s">
         <v>1000</v>
       </c>
@@ -17136,7 +17169,7 @@
       </c>
       <c r="H197" s="4"/>
     </row>
-    <row r="198" spans="1:8" ht="409.5">
+    <row r="198" spans="1:8" ht="409.6">
       <c r="A198" s="6" t="s">
         <v>1005</v>
       </c>
@@ -17160,7 +17193,7 @@
       </c>
       <c r="H198" s="4"/>
     </row>
-    <row r="199" spans="1:8" ht="409.5">
+    <row r="199" spans="1:8" ht="409.6">
       <c r="A199" s="7" t="s">
         <v>1010</v>
       </c>
@@ -17184,7 +17217,7 @@
       </c>
       <c r="H199" s="4"/>
     </row>
-    <row r="200" spans="1:8" ht="409.5">
+    <row r="200" spans="1:8" ht="409.6">
       <c r="A200" s="6" t="s">
         <v>1015</v>
       </c>
@@ -17208,7 +17241,7 @@
       </c>
       <c r="H200" s="4"/>
     </row>
-    <row r="201" spans="1:8" ht="358.8">
+    <row r="201" spans="1:8" ht="388">
       <c r="A201" s="6" t="s">
         <v>1021</v>
       </c>

</xml_diff>